<commit_message>
On branch master - updated method to split-out label from file name
Changes to be committed:
	modified:   classify-pet-images/get_pet_labels.py
	modified:   classify-pet-images/pet-images_alexnet.txt
	modified:   classify-pet-images/pet-images_resnet.txt
	modified:   classify-pet-images/pet-images_vgg.txt
	modified:   pre-trained image classifier results.xlsx
</commit_message>
<xml_diff>
--- a/pre-trained image classifier results.xlsx
+++ b/pre-trained image classifier results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyScripts\udacity\python\ai\p1_dog_classifier\revision\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2008F427-28D0-4565-A785-679996D484DB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC1380E-F225-4A9E-B79F-C6BC550140EF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14625" windowHeight="11295" firstSheet="4" activeTab="4" xr2:uid="{9EA02F68-53A7-46B5-86B7-426B714E97B8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14625" windowHeight="11295" firstSheet="5" activeTab="7" xr2:uid="{9EA02F68-53A7-46B5-86B7-426B714E97B8}"/>
   </bookViews>
   <sheets>
     <sheet name="resnet" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="adj_results_vgg" sheetId="5" r:id="rId5"/>
     <sheet name="adj_results_resnet" sheetId="6" r:id="rId6"/>
     <sheet name="adj_results_alexnet" sheetId="7" r:id="rId7"/>
+    <sheet name="submit#2" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="271">
   <si>
     <t>Command Line Arguments:</t>
   </si>
@@ -893,12 +894,126 @@
   <si>
     <t xml:space="preserve">Run time (seconds): </t>
   </si>
+  <si>
+    <t>Sent to Udacity Support:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I am deeply offended by the accusation of plagiarism in my submission of project 1. Especially as I cited the source in a comment. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Plagiarism as defined by Udacity: "Plagiarism at Udacity can range from submitting a project you didn’t create to copying code into a program </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>without citation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>." Emphasis is mine.</t>
+    </r>
+  </si>
+  <si>
+    <t>Original code (get_pet_labels.py) - comment and line of code highlighted below:</t>
+  </si>
+  <si>
+    <t>    list_of_filenames = listdir(image_dir)</t>
+  </si>
+  <si>
+    <t>    results_dic = dict()</t>
+  </si>
+  <si>
+    <t>    for i in range(0, len(list_of_filenames), 1):</t>
+  </si>
+  <si>
+    <t>      if list_of_filenames[i] not in results_dic:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t># found solution to remove digits at</t>
+    </r>
+  </si>
+  <si>
+    <t>          # https://stackoverflow.com/questions/12851791/removing-numbers-from-string</t>
+  </si>
+  <si>
+    <t>          pet_label = ''.join([j for j in list_of_filenames[i] if not j.isdigit()])</t>
+  </si>
+  <si>
+    <t>          # get rid of any underscores</t>
+  </si>
+  <si>
+    <t>          pet_label = pet_label.replace('_', ' ')</t>
+  </si>
+  <si>
+    <t>          # remove extension [:-4], strip whitespace, make lowercase</t>
+  </si>
+  <si>
+    <t>          results_dic[list_of_filenames[i]] = [pet_label[:-4].strip().lower()]</t>
+  </si>
+  <si>
+    <t>      else:</t>
+  </si>
+  <si>
+    <t>          print("Warning: Key={} already exist in results_dic with value = {}".</t>
+  </si>
+  <si>
+    <t>            format(list_of_filenames[i], results_dic[list_of_filenames[i]]))</t>
+  </si>
+  <si>
+    <t>    return results_dic</t>
+  </si>
+  <si>
+    <t>Note the citation in the comments as per the Udacity guidelines. It makes me wonder if the reviewer would even have known the above line was used elsewhere if not for the comment I inserted. Furthermore, it calls into question whether the reviewer understands the guidelines for what constitutes plagiarism. Seriously, if I were going to plagiarize would I put a comment in my code indicating I found similar code elsewhere?</t>
+  </si>
+  <si>
+    <t>As this is not the first Nanodegree for me the subject has come up before and based on comments from the Udacity Community Managers in Slack what I did above was acceptable and within established guidelines.</t>
+  </si>
+  <si>
+    <t>If the guidelines as stated on Udacity's site are ambiguous or subject to interpretation then it is up to Udacity to clarify them and ensure their reviewers understand them. In fact, common problems often have common solutions. Evidence from the reviewer's suggestion to follow a certain method to solve the problem.</t>
+  </si>
+  <si>
+    <t>If what the reviewer is really concerned about is finding the best possible solution to solve the problem. Well, I have no problem with that and their encouraging or suggesting another solution that may be better is welcome. What is not welcome is blatantly accusing someone of plagiarism.</t>
+  </si>
+  <si>
+    <t>Take note that I modified my solution and resubmitted my project even though my solution did work given the stated requirements.</t>
+  </si>
+  <si>
+    <t>Thank you</t>
+  </si>
+  <si>
+    <t>https://udacity.zendesk.com/hc/en-us/articles/360001451091-What-is-plagiarism-</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="9"/>
       <color theme="1"/>
@@ -944,13 +1059,58 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Arial Rounded MT Bold"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -1040,11 +1200,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1093,9 +1254,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1105,11 +1263,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -3871,9 +4046,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC57D9E9-5B08-4C2E-82F0-8AC61EEED1BE}">
   <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -3974,43 +4149,43 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="26" t="s">
         <v>185</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="H9" s="30" t="s">
+      <c r="H9" s="29" t="s">
         <v>172</v>
       </c>
-      <c r="I9" s="30" t="s">
+      <c r="I9" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="J9" s="30" t="s">
+      <c r="J9" s="29" t="s">
         <v>174</v>
       </c>
-      <c r="K9" s="31" t="s">
+      <c r="K9" s="30" t="s">
         <v>210</v>
       </c>
-      <c r="L9" s="31" t="s">
+      <c r="L9" s="30" t="s">
         <v>211</v>
       </c>
-      <c r="M9" s="31" t="s">
+      <c r="M9" s="30" t="s">
         <v>212</v>
       </c>
     </row>
@@ -5591,7 +5766,7 @@
       <c r="G60" s="25" t="s">
         <v>225</v>
       </c>
-      <c r="H60" s="26">
+      <c r="H60" s="31">
         <f>H53 / H54</f>
         <v>1</v>
       </c>
@@ -5600,7 +5775,7 @@
       <c r="G61" s="25" t="s">
         <v>226</v>
       </c>
-      <c r="H61" s="26">
+      <c r="H61" s="31">
         <f>H55 / H56</f>
         <v>1</v>
       </c>
@@ -5609,7 +5784,7 @@
       <c r="G62" s="25" t="s">
         <v>227</v>
       </c>
-      <c r="H62" s="32">
+      <c r="H62" s="31">
         <f>H57 / H54</f>
         <v>0.93333333333333335</v>
       </c>
@@ -5618,7 +5793,7 @@
       <c r="G63" s="25" t="s">
         <v>228</v>
       </c>
-      <c r="H63" s="26">
+      <c r="H63" s="31">
         <f>H58 / H52</f>
         <v>0.875</v>
       </c>
@@ -5648,7 +5823,7 @@
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G72" sqref="G72"/>
+      <selection pane="bottomLeft" activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -5750,43 +5925,43 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="26" t="s">
         <v>185</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="H9" s="30" t="s">
+      <c r="H9" s="29" t="s">
         <v>172</v>
       </c>
-      <c r="I9" s="30" t="s">
+      <c r="I9" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="J9" s="30" t="s">
+      <c r="J9" s="29" t="s">
         <v>174</v>
       </c>
-      <c r="K9" s="31" t="s">
+      <c r="K9" s="30" t="s">
         <v>210</v>
       </c>
-      <c r="L9" s="31" t="s">
+      <c r="L9" s="30" t="s">
         <v>211</v>
       </c>
-      <c r="M9" s="31" t="s">
+      <c r="M9" s="30" t="s">
         <v>212</v>
       </c>
     </row>
@@ -7370,7 +7545,7 @@
       <c r="G60" s="25" t="s">
         <v>225</v>
       </c>
-      <c r="H60" s="26">
+      <c r="H60" s="31">
         <f>H53 / H54</f>
         <v>1</v>
       </c>
@@ -7379,7 +7554,7 @@
       <c r="G61" s="25" t="s">
         <v>226</v>
       </c>
-      <c r="H61" s="26">
+      <c r="H61" s="31">
         <f>H55 / H56</f>
         <v>1</v>
       </c>
@@ -7388,7 +7563,7 @@
       <c r="G62" s="25" t="s">
         <v>227</v>
       </c>
-      <c r="H62" s="26">
+      <c r="H62" s="31">
         <f>H57 / H54</f>
         <v>0.9</v>
       </c>
@@ -7397,7 +7572,7 @@
       <c r="G63" s="25" t="s">
         <v>228</v>
       </c>
-      <c r="H63" s="26">
+      <c r="H63" s="31">
         <f>H58 / H52</f>
         <v>0.82499999999999996</v>
       </c>
@@ -7498,8 +7673,8 @@
   <dimension ref="A1:M65"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H66" sqref="H66"/>
+      <pane ySplit="9" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -7599,43 +7774,43 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="26" t="s">
         <v>185</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="H9" s="30" t="s">
+      <c r="H9" s="29" t="s">
         <v>172</v>
       </c>
-      <c r="I9" s="30" t="s">
+      <c r="I9" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="J9" s="30" t="s">
+      <c r="J9" s="29" t="s">
         <v>174</v>
       </c>
-      <c r="K9" s="31" t="s">
+      <c r="K9" s="30" t="s">
         <v>210</v>
       </c>
-      <c r="L9" s="31" t="s">
+      <c r="L9" s="30" t="s">
         <v>211</v>
       </c>
-      <c r="M9" s="31" t="s">
+      <c r="M9" s="30" t="s">
         <v>212</v>
       </c>
     </row>
@@ -9211,7 +9386,7 @@
       <c r="G60" s="25" t="s">
         <v>225</v>
       </c>
-      <c r="H60" s="26">
+      <c r="H60" s="31">
         <f>H53 / H54</f>
         <v>1</v>
       </c>
@@ -9220,7 +9395,7 @@
       <c r="G61" s="25" t="s">
         <v>226</v>
       </c>
-      <c r="H61" s="26">
+      <c r="H61" s="31">
         <f>H55 / H56</f>
         <v>1</v>
       </c>
@@ -9229,7 +9404,7 @@
       <c r="G62" s="25" t="s">
         <v>227</v>
       </c>
-      <c r="H62" s="26">
+      <c r="H62" s="31">
         <f>H57 / H54</f>
         <v>0.8</v>
       </c>
@@ -9238,7 +9413,7 @@
       <c r="G63" s="25" t="s">
         <v>228</v>
       </c>
-      <c r="H63" s="26">
+      <c r="H63" s="31">
         <f>H58 / H52</f>
         <v>0.75</v>
       </c>
@@ -9254,4 +9429,185 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C51C57-0ABB-43F3-AD4D-83D65618082C}">
+  <dimension ref="A1:A37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="83.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="37" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="33" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="33"/>
+    </row>
+    <row r="5" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="33" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="33"/>
+    </row>
+    <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="33" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="32"/>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="34" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="34" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="34" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="34" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="34" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="35" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="35" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="34" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="34" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="34" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="34" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="34" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="34" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="34" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="34" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="33"/>
+    </row>
+    <row r="25" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="33" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="33"/>
+    </row>
+    <row r="27" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="33" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="33"/>
+    </row>
+    <row r="29" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="33" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="33"/>
+    </row>
+    <row r="31" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="33" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="33"/>
+    </row>
+    <row r="33" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="33" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="33"/>
+    </row>
+    <row r="35" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="33" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="33"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="36" t="s">
+        <v>270</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A37" r:id="rId1" xr:uid="{E94C0CB4-183C-4C28-8633-2A3B481BB114}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>